<commit_message>
minor update to code to imporve automation
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/C-path/TOMI 2/CHAOS Index/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/C-path/TOMI 2/CHAOS Index/CHAOSpackage/CHAOSindex/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87469FCF-AC7B-4C4A-AF29-54A13CA309AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1F9AA4-1D61-5649-82E4-B71D6E22AC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2320" windowWidth="22960" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
+    <workbookView xWindow="2580" yWindow="1780" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_GoBack" localSheetId="0">Sheet1!$A$12</definedName>
+    <definedName name="_GoBack" localSheetId="0">Sheet1!$A$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t>old_vars</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>dexcomg4</t>
+  </si>
+  <si>
+    <t>serial_number</t>
+  </si>
+  <si>
+    <t>meter_timestamp</t>
+  </si>
+  <si>
+    <t>record_type</t>
+  </si>
+  <si>
+    <t>historic_glucose_mmol_l</t>
+  </si>
+  <si>
+    <t>scan_glucose_mmol_L</t>
   </si>
 </sst>
 </file>
@@ -524,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,10 +563,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
@@ -559,7 +574,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -570,10 +585,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -581,10 +596,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -592,10 +607,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -603,10 +618,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -614,10 +629,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
@@ -625,10 +640,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -636,21 +651,21 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -658,10 +673,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
@@ -669,10 +684,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -680,32 +695,32 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
+      <c r="A15" t="s">
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -713,10 +728,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -724,10 +739,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -735,10 +750,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -746,10 +761,10 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
@@ -757,10 +772,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
@@ -768,10 +783,10 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
@@ -779,10 +794,10 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
@@ -790,10 +805,10 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -801,73 +816,125 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>32</v>
+      <c r="A26" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
       </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>37</v>
+      <c r="A29" t="s">
+        <v>41</v>
       </c>
       <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="C29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>